<commit_message>
separate functions out from menu_popup.js
</commit_message>
<xml_diff>
--- a/gardenContent/gardenContent.xlsx
+++ b/gardenContent/gardenContent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hu/Documents/CarolinaCloudApp/EdibleGardenUNC/gardenContent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9591BD-E9D0-2946-A4E3-25603678DE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD53576-9277-F946-95DC-AE176C00829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14060" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13980" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Garden" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t>plantName</t>
   </si>
@@ -62,9 +62,6 @@
     <t>tomato_lenoir</t>
   </si>
   <si>
-    <t>tomato_main</t>
-  </si>
-  <si>
     <t>tomato_stacy</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>Spinach_fetzer</t>
-  </si>
-  <si>
-    <t>Spinach_main</t>
   </si>
   <si>
     <t>Rosemary</t>
@@ -333,6 +327,51 @@
   </si>
   <si>
     <t>Onion</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/GtF3gQ83/phillip-larking-alnk961d-Nz8-unsplash.jpg</t>
+  </si>
+  <si>
+    <t>Cilantro</t>
+  </si>
+  <si>
+    <t>Cut leaves from the top of the plant when they are 4-6 inches tall.</t>
+  </si>
+  <si>
+    <t>Easy Cilantro-Lime Rice
+Ingredients
+1 tablespoon olive oil
+1 cup basmati rice
+2 cloves garlic, minced
+1 ½ cups chicken broth
+2 tablespoons fresh lime juice
+1 teaspoon salt
+½ cup chopped cilantro
+¼ cup whole-kernel corn
+2 teaspoons green onions, chopped
+1 lime, zested
+Directions
+Heat olive oil in a saucepan over medium heat. Cook and stir rice and garlic in hot oil until fragrant, about 2 minutes. Stir chicken broth, lime juice, and salt into rice; bring to a boil, reduce heat to medium-low, cover the saucepan with a lid, and simmer until rice is tender and liquid is absorbed, about 15 minutes.
+Stir cilantro, corn, green onions, and lime zest into rice until well-mixed.</t>
+  </si>
+  <si>
+    <t>Cilantro Garlic Lime Sauteed Shrimp
+Ingredients
+1 ½ pounds shrimp, tails removed
+1 bunch fresh cilantro, chopped, or to taste, divided
+¼ cup olive oil
+½ yellow onion, chopped
+5 cloves garlic, chopped, or more to taste
+2 cups salsa
+1 red bell pepper, finely chopped
+¾ cup white wine
+1 small red chile pepper, pureed
+1 teaspoon lemon juice, or to taste
+1 teaspoon lime juice, or to taste
+Directions
+Toss shrimp and half the cilantro together in a bowl.
+Heat olive oil in a skillet over medium heat; saute onion until translucent, 1 to 2 minutes. Add garlic and saute until browned, 1 to 2 minutes.
+Stir salsa, red bell pepper, white wine, red chile pepper puree, lemon juice, and lime juice into onion mixture; bring to a boil. Reduce heat and simmer, 2 to 3 minutes. Add shrimp to salsa mixture; cook and stir until shrimp are cooked through, about 5 minutes. Garnish with remaining cilantro and add more lemon or lime juice to taste.</t>
   </si>
 </sst>
 </file>
@@ -664,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -698,78 +737,114 @@
     </row>
     <row r="2" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="365" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="395" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{BFC0B66C-FE68-4F72-87AF-82EB78BFFC8E}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{42D26DAD-8D43-4C09-80F4-A5ED207D79ED}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{0C2C5254-52FA-40C3-99BF-B14264DE2666}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{3B10480F-009C-47CE-A769-1D3699892258}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{0C2C5254-52FA-40C3-99BF-B14264DE2666}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{3B10480F-009C-47CE-A769-1D3699892258}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{DFB9C77B-0E43-418C-925E-D70B15770260}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{142E9A71-0BF2-4BFF-9471-003B562783B8}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{5C832106-29B3-D848-BA6F-D9EE4BC9EA7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -780,7 +855,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -811,19 +886,19 @@
     </row>
     <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -831,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -888,19 +963,19 @@
     </row>
     <row r="2" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +1016,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -969,7 +1044,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,19 +1075,19 @@
     </row>
     <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1052,10 +1127,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1104,10 +1179,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1156,10 +1231,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1183,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA00F31-40E4-4EF3-AE2A-3CBC71618EFA}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1215,27 +1290,27 @@
     </row>
     <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>

</xml_diff>